<commit_message>
predict for ensemble output as pickle
</commit_message>
<xml_diff>
--- a/data/log.xlsx
+++ b/data/log.xlsx
@@ -197,8 +197,8 @@
   </sheetPr>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -622,6 +622,24 @@
       </c>
       <c r="C35" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>0.9004</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>0.6717</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>0.9009</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v>0.7082</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>